<commit_message>
created basic API methods
</commit_message>
<xml_diff>
--- a/files/output/result_Islington_2025_05_17.xlsx
+++ b/files/output/result_Islington_2025_05_17.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21500" windowHeight="11100" activeTab="1"/>
+    <workbookView windowWidth="28060" windowHeight="11100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -9382,10 +9382,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
@@ -9412,17 +9412,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9436,96 +9429,12 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -9542,7 +9451,98 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9557,7 +9557,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9569,97 +9689,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9671,43 +9719,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9719,25 +9731,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9748,21 +9748,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -9790,26 +9775,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9848,123 +9824,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -9973,25 +9973,25 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -23581,7 +23581,1019 @@
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" autoFormatId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" createdVersion="5" useAutoFormatting="1" compact="0" indent="0" outline="1" compactData="0" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:H10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
-    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0">
+      <items count="1009">
+        <item x="0"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="229"/>
+        <item x="230"/>
+        <item x="231"/>
+        <item x="232"/>
+        <item x="233"/>
+        <item x="234"/>
+        <item x="235"/>
+        <item x="236"/>
+        <item x="237"/>
+        <item x="221"/>
+        <item x="238"/>
+        <item x="239"/>
+        <item x="240"/>
+        <item x="241"/>
+        <item x="242"/>
+        <item x="243"/>
+        <item x="222"/>
+        <item x="223"/>
+        <item x="224"/>
+        <item x="225"/>
+        <item x="226"/>
+        <item x="227"/>
+        <item x="228"/>
+        <item x="244"/>
+        <item x="253"/>
+        <item x="254"/>
+        <item x="255"/>
+        <item x="256"/>
+        <item x="257"/>
+        <item x="258"/>
+        <item x="259"/>
+        <item x="260"/>
+        <item x="261"/>
+        <item x="262"/>
+        <item x="245"/>
+        <item x="263"/>
+        <item x="264"/>
+        <item x="265"/>
+        <item x="266"/>
+        <item x="267"/>
+        <item x="268"/>
+        <item x="246"/>
+        <item x="247"/>
+        <item x="248"/>
+        <item x="249"/>
+        <item x="250"/>
+        <item x="251"/>
+        <item x="252"/>
+        <item x="269"/>
+        <item x="278"/>
+        <item x="279"/>
+        <item x="280"/>
+        <item x="281"/>
+        <item x="282"/>
+        <item x="283"/>
+        <item x="284"/>
+        <item x="285"/>
+        <item x="286"/>
+        <item x="270"/>
+        <item x="287"/>
+        <item x="288"/>
+        <item x="289"/>
+        <item x="290"/>
+        <item x="291"/>
+        <item x="292"/>
+        <item x="271"/>
+        <item x="272"/>
+        <item x="273"/>
+        <item x="274"/>
+        <item x="275"/>
+        <item x="276"/>
+        <item x="277"/>
+        <item x="293"/>
+        <item x="302"/>
+        <item x="303"/>
+        <item x="304"/>
+        <item x="305"/>
+        <item x="306"/>
+        <item x="307"/>
+        <item x="308"/>
+        <item x="309"/>
+        <item x="310"/>
+        <item x="311"/>
+        <item x="294"/>
+        <item x="312"/>
+        <item x="313"/>
+        <item x="314"/>
+        <item x="315"/>
+        <item x="316"/>
+        <item x="317"/>
+        <item x="295"/>
+        <item x="296"/>
+        <item x="297"/>
+        <item x="298"/>
+        <item x="299"/>
+        <item x="300"/>
+        <item x="301"/>
+        <item x="325"/>
+        <item x="326"/>
+        <item x="327"/>
+        <item x="328"/>
+        <item x="329"/>
+        <item x="330"/>
+        <item x="331"/>
+        <item x="332"/>
+        <item x="333"/>
+        <item x="334"/>
+        <item x="318"/>
+        <item x="335"/>
+        <item x="336"/>
+        <item x="337"/>
+        <item x="338"/>
+        <item x="339"/>
+        <item x="340"/>
+        <item x="319"/>
+        <item x="320"/>
+        <item x="321"/>
+        <item x="322"/>
+        <item x="323"/>
+        <item x="324"/>
+        <item x="349"/>
+        <item x="350"/>
+        <item x="351"/>
+        <item x="352"/>
+        <item x="353"/>
+        <item x="354"/>
+        <item x="355"/>
+        <item x="356"/>
+        <item x="357"/>
+        <item x="358"/>
+        <item x="341"/>
+        <item x="359"/>
+        <item x="360"/>
+        <item x="361"/>
+        <item x="362"/>
+        <item x="363"/>
+        <item x="364"/>
+        <item x="342"/>
+        <item x="343"/>
+        <item x="344"/>
+        <item x="345"/>
+        <item x="346"/>
+        <item x="347"/>
+        <item x="348"/>
+        <item x="373"/>
+        <item x="374"/>
+        <item x="375"/>
+        <item x="376"/>
+        <item x="377"/>
+        <item x="378"/>
+        <item x="379"/>
+        <item x="380"/>
+        <item x="381"/>
+        <item x="382"/>
+        <item x="365"/>
+        <item x="383"/>
+        <item x="384"/>
+        <item x="385"/>
+        <item x="386"/>
+        <item x="387"/>
+        <item x="388"/>
+        <item x="366"/>
+        <item x="367"/>
+        <item x="368"/>
+        <item x="369"/>
+        <item x="370"/>
+        <item x="371"/>
+        <item x="372"/>
+        <item x="397"/>
+        <item x="398"/>
+        <item x="399"/>
+        <item x="400"/>
+        <item x="401"/>
+        <item x="402"/>
+        <item x="403"/>
+        <item x="404"/>
+        <item x="405"/>
+        <item x="406"/>
+        <item x="389"/>
+        <item x="407"/>
+        <item x="408"/>
+        <item x="409"/>
+        <item x="410"/>
+        <item x="411"/>
+        <item x="412"/>
+        <item x="390"/>
+        <item x="391"/>
+        <item x="392"/>
+        <item x="393"/>
+        <item x="394"/>
+        <item x="395"/>
+        <item x="396"/>
+        <item x="421"/>
+        <item x="422"/>
+        <item x="423"/>
+        <item x="424"/>
+        <item x="425"/>
+        <item x="426"/>
+        <item x="427"/>
+        <item x="428"/>
+        <item x="429"/>
+        <item x="430"/>
+        <item x="413"/>
+        <item x="431"/>
+        <item x="432"/>
+        <item x="433"/>
+        <item x="434"/>
+        <item x="435"/>
+        <item x="436"/>
+        <item x="414"/>
+        <item x="415"/>
+        <item x="416"/>
+        <item x="417"/>
+        <item x="418"/>
+        <item x="419"/>
+        <item x="420"/>
+        <item x="443"/>
+        <item x="444"/>
+        <item x="445"/>
+        <item x="446"/>
+        <item x="447"/>
+        <item x="448"/>
+        <item x="449"/>
+        <item x="450"/>
+        <item x="451"/>
+        <item x="452"/>
+        <item x="437"/>
+        <item x="453"/>
+        <item x="454"/>
+        <item x="455"/>
+        <item x="456"/>
+        <item x="457"/>
+        <item x="458"/>
+        <item x="438"/>
+        <item x="439"/>
+        <item x="440"/>
+        <item x="441"/>
+        <item x="442"/>
+        <item x="25"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="26"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="459"/>
+        <item x="468"/>
+        <item x="469"/>
+        <item x="470"/>
+        <item x="471"/>
+        <item x="472"/>
+        <item x="473"/>
+        <item x="474"/>
+        <item x="475"/>
+        <item x="476"/>
+        <item x="477"/>
+        <item x="460"/>
+        <item x="478"/>
+        <item x="479"/>
+        <item x="480"/>
+        <item x="481"/>
+        <item x="482"/>
+        <item x="483"/>
+        <item x="461"/>
+        <item x="462"/>
+        <item x="463"/>
+        <item x="464"/>
+        <item x="465"/>
+        <item x="466"/>
+        <item x="467"/>
+        <item x="484"/>
+        <item x="493"/>
+        <item x="494"/>
+        <item x="495"/>
+        <item x="496"/>
+        <item x="497"/>
+        <item x="498"/>
+        <item x="499"/>
+        <item x="500"/>
+        <item x="501"/>
+        <item x="502"/>
+        <item x="485"/>
+        <item x="503"/>
+        <item x="504"/>
+        <item x="505"/>
+        <item x="506"/>
+        <item x="507"/>
+        <item x="508"/>
+        <item x="486"/>
+        <item x="487"/>
+        <item x="488"/>
+        <item x="489"/>
+        <item x="490"/>
+        <item x="491"/>
+        <item x="492"/>
+        <item x="516"/>
+        <item x="517"/>
+        <item x="518"/>
+        <item x="519"/>
+        <item x="520"/>
+        <item x="521"/>
+        <item x="522"/>
+        <item x="523"/>
+        <item x="524"/>
+        <item x="525"/>
+        <item x="509"/>
+        <item x="526"/>
+        <item x="527"/>
+        <item x="528"/>
+        <item x="529"/>
+        <item x="530"/>
+        <item x="531"/>
+        <item x="510"/>
+        <item x="511"/>
+        <item x="512"/>
+        <item x="513"/>
+        <item x="514"/>
+        <item x="515"/>
+        <item x="540"/>
+        <item x="541"/>
+        <item x="542"/>
+        <item x="543"/>
+        <item x="544"/>
+        <item x="545"/>
+        <item x="546"/>
+        <item x="547"/>
+        <item x="548"/>
+        <item x="549"/>
+        <item x="532"/>
+        <item x="550"/>
+        <item x="551"/>
+        <item x="552"/>
+        <item x="553"/>
+        <item x="554"/>
+        <item x="555"/>
+        <item x="533"/>
+        <item x="534"/>
+        <item x="535"/>
+        <item x="536"/>
+        <item x="537"/>
+        <item x="538"/>
+        <item x="539"/>
+        <item x="564"/>
+        <item x="565"/>
+        <item x="566"/>
+        <item x="567"/>
+        <item x="568"/>
+        <item x="569"/>
+        <item x="570"/>
+        <item x="571"/>
+        <item x="572"/>
+        <item x="556"/>
+        <item x="573"/>
+        <item x="574"/>
+        <item x="575"/>
+        <item x="576"/>
+        <item x="577"/>
+        <item x="578"/>
+        <item x="557"/>
+        <item x="558"/>
+        <item x="559"/>
+        <item x="560"/>
+        <item x="561"/>
+        <item x="562"/>
+        <item x="563"/>
+        <item x="579"/>
+        <item x="588"/>
+        <item x="589"/>
+        <item x="590"/>
+        <item x="591"/>
+        <item x="592"/>
+        <item x="593"/>
+        <item x="594"/>
+        <item x="595"/>
+        <item x="596"/>
+        <item x="597"/>
+        <item x="580"/>
+        <item x="598"/>
+        <item x="599"/>
+        <item x="600"/>
+        <item x="601"/>
+        <item x="602"/>
+        <item x="603"/>
+        <item x="581"/>
+        <item x="582"/>
+        <item x="583"/>
+        <item x="584"/>
+        <item x="585"/>
+        <item x="586"/>
+        <item x="587"/>
+        <item x="612"/>
+        <item x="613"/>
+        <item x="614"/>
+        <item x="615"/>
+        <item x="616"/>
+        <item x="617"/>
+        <item x="618"/>
+        <item x="619"/>
+        <item x="620"/>
+        <item x="621"/>
+        <item x="604"/>
+        <item x="622"/>
+        <item x="623"/>
+        <item x="624"/>
+        <item x="625"/>
+        <item x="626"/>
+        <item x="627"/>
+        <item x="605"/>
+        <item x="606"/>
+        <item x="607"/>
+        <item x="608"/>
+        <item x="609"/>
+        <item x="610"/>
+        <item x="611"/>
+        <item x="636"/>
+        <item x="637"/>
+        <item x="638"/>
+        <item x="639"/>
+        <item x="640"/>
+        <item x="641"/>
+        <item x="642"/>
+        <item x="643"/>
+        <item x="644"/>
+        <item x="645"/>
+        <item x="628"/>
+        <item x="646"/>
+        <item x="647"/>
+        <item x="648"/>
+        <item x="649"/>
+        <item x="650"/>
+        <item x="651"/>
+        <item x="629"/>
+        <item x="630"/>
+        <item x="631"/>
+        <item x="632"/>
+        <item x="633"/>
+        <item x="634"/>
+        <item x="635"/>
+        <item x="660"/>
+        <item x="661"/>
+        <item x="662"/>
+        <item x="663"/>
+        <item x="664"/>
+        <item x="665"/>
+        <item x="666"/>
+        <item x="667"/>
+        <item x="668"/>
+        <item x="669"/>
+        <item x="652"/>
+        <item x="670"/>
+        <item x="671"/>
+        <item x="672"/>
+        <item x="673"/>
+        <item x="674"/>
+        <item x="675"/>
+        <item x="653"/>
+        <item x="654"/>
+        <item x="655"/>
+        <item x="656"/>
+        <item x="657"/>
+        <item x="658"/>
+        <item x="659"/>
+        <item x="684"/>
+        <item x="685"/>
+        <item x="686"/>
+        <item x="687"/>
+        <item x="688"/>
+        <item x="689"/>
+        <item x="690"/>
+        <item x="691"/>
+        <item x="692"/>
+        <item x="693"/>
+        <item x="676"/>
+        <item x="694"/>
+        <item x="695"/>
+        <item x="696"/>
+        <item x="697"/>
+        <item x="698"/>
+        <item x="699"/>
+        <item x="677"/>
+        <item x="678"/>
+        <item x="679"/>
+        <item x="680"/>
+        <item x="681"/>
+        <item x="682"/>
+        <item x="683"/>
+        <item x="50"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="51"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="708"/>
+        <item x="709"/>
+        <item x="710"/>
+        <item x="711"/>
+        <item x="712"/>
+        <item x="713"/>
+        <item x="714"/>
+        <item x="715"/>
+        <item x="716"/>
+        <item x="717"/>
+        <item x="700"/>
+        <item x="718"/>
+        <item x="719"/>
+        <item x="720"/>
+        <item x="721"/>
+        <item x="722"/>
+        <item x="723"/>
+        <item x="701"/>
+        <item x="702"/>
+        <item x="703"/>
+        <item x="704"/>
+        <item x="705"/>
+        <item x="706"/>
+        <item x="707"/>
+        <item x="724"/>
+        <item x="733"/>
+        <item x="734"/>
+        <item x="735"/>
+        <item x="736"/>
+        <item x="737"/>
+        <item x="738"/>
+        <item x="739"/>
+        <item x="740"/>
+        <item x="741"/>
+        <item x="742"/>
+        <item x="725"/>
+        <item x="743"/>
+        <item x="744"/>
+        <item x="745"/>
+        <item x="746"/>
+        <item x="747"/>
+        <item x="748"/>
+        <item x="726"/>
+        <item x="727"/>
+        <item x="728"/>
+        <item x="729"/>
+        <item x="730"/>
+        <item x="731"/>
+        <item x="732"/>
+        <item x="757"/>
+        <item x="758"/>
+        <item x="759"/>
+        <item x="760"/>
+        <item x="761"/>
+        <item x="762"/>
+        <item x="763"/>
+        <item x="764"/>
+        <item x="765"/>
+        <item x="766"/>
+        <item x="749"/>
+        <item x="767"/>
+        <item x="768"/>
+        <item x="769"/>
+        <item x="770"/>
+        <item x="771"/>
+        <item x="772"/>
+        <item x="750"/>
+        <item x="751"/>
+        <item x="752"/>
+        <item x="753"/>
+        <item x="754"/>
+        <item x="755"/>
+        <item x="756"/>
+        <item x="781"/>
+        <item x="782"/>
+        <item x="783"/>
+        <item x="784"/>
+        <item x="785"/>
+        <item x="786"/>
+        <item x="787"/>
+        <item x="788"/>
+        <item x="789"/>
+        <item x="790"/>
+        <item x="773"/>
+        <item x="791"/>
+        <item x="792"/>
+        <item x="793"/>
+        <item x="794"/>
+        <item x="795"/>
+        <item x="796"/>
+        <item x="774"/>
+        <item x="775"/>
+        <item x="776"/>
+        <item x="777"/>
+        <item x="778"/>
+        <item x="779"/>
+        <item x="780"/>
+        <item x="805"/>
+        <item x="806"/>
+        <item x="807"/>
+        <item x="808"/>
+        <item x="809"/>
+        <item x="810"/>
+        <item x="811"/>
+        <item x="812"/>
+        <item x="813"/>
+        <item x="797"/>
+        <item x="814"/>
+        <item x="815"/>
+        <item x="816"/>
+        <item x="817"/>
+        <item x="818"/>
+        <item x="819"/>
+        <item x="798"/>
+        <item x="799"/>
+        <item x="800"/>
+        <item x="801"/>
+        <item x="802"/>
+        <item x="803"/>
+        <item x="804"/>
+        <item x="828"/>
+        <item x="829"/>
+        <item x="830"/>
+        <item x="831"/>
+        <item x="832"/>
+        <item x="833"/>
+        <item x="834"/>
+        <item x="835"/>
+        <item x="836"/>
+        <item x="820"/>
+        <item x="837"/>
+        <item x="838"/>
+        <item x="839"/>
+        <item x="840"/>
+        <item x="841"/>
+        <item x="842"/>
+        <item x="821"/>
+        <item x="822"/>
+        <item x="823"/>
+        <item x="824"/>
+        <item x="825"/>
+        <item x="826"/>
+        <item x="827"/>
+        <item x="851"/>
+        <item x="852"/>
+        <item x="853"/>
+        <item x="854"/>
+        <item x="855"/>
+        <item x="856"/>
+        <item x="857"/>
+        <item x="858"/>
+        <item x="859"/>
+        <item x="860"/>
+        <item x="843"/>
+        <item x="861"/>
+        <item x="862"/>
+        <item x="863"/>
+        <item x="864"/>
+        <item x="865"/>
+        <item x="866"/>
+        <item x="844"/>
+        <item x="845"/>
+        <item x="846"/>
+        <item x="847"/>
+        <item x="848"/>
+        <item x="849"/>
+        <item x="850"/>
+        <item x="875"/>
+        <item x="876"/>
+        <item x="877"/>
+        <item x="878"/>
+        <item x="879"/>
+        <item x="880"/>
+        <item x="881"/>
+        <item x="882"/>
+        <item x="883"/>
+        <item x="867"/>
+        <item x="884"/>
+        <item x="885"/>
+        <item x="886"/>
+        <item x="887"/>
+        <item x="888"/>
+        <item x="868"/>
+        <item x="869"/>
+        <item x="870"/>
+        <item x="871"/>
+        <item x="872"/>
+        <item x="873"/>
+        <item x="874"/>
+        <item x="897"/>
+        <item x="898"/>
+        <item x="899"/>
+        <item x="900"/>
+        <item x="901"/>
+        <item x="902"/>
+        <item x="903"/>
+        <item x="904"/>
+        <item x="905"/>
+        <item x="906"/>
+        <item x="889"/>
+        <item x="907"/>
+        <item x="908"/>
+        <item x="909"/>
+        <item x="910"/>
+        <item x="911"/>
+        <item x="912"/>
+        <item x="890"/>
+        <item x="891"/>
+        <item x="892"/>
+        <item x="893"/>
+        <item x="894"/>
+        <item x="895"/>
+        <item x="896"/>
+        <item x="920"/>
+        <item x="921"/>
+        <item x="922"/>
+        <item x="923"/>
+        <item x="924"/>
+        <item x="925"/>
+        <item x="926"/>
+        <item x="927"/>
+        <item x="928"/>
+        <item x="929"/>
+        <item x="930"/>
+        <item x="931"/>
+        <item x="932"/>
+        <item x="933"/>
+        <item x="934"/>
+        <item x="935"/>
+        <item x="913"/>
+        <item x="914"/>
+        <item x="915"/>
+        <item x="916"/>
+        <item x="917"/>
+        <item x="918"/>
+        <item x="919"/>
+        <item x="75"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="76"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="944"/>
+        <item x="945"/>
+        <item x="946"/>
+        <item x="947"/>
+        <item x="948"/>
+        <item x="949"/>
+        <item x="950"/>
+        <item x="951"/>
+        <item x="952"/>
+        <item x="953"/>
+        <item x="936"/>
+        <item x="954"/>
+        <item x="955"/>
+        <item x="956"/>
+        <item x="957"/>
+        <item x="958"/>
+        <item x="959"/>
+        <item x="937"/>
+        <item x="938"/>
+        <item x="939"/>
+        <item x="940"/>
+        <item x="941"/>
+        <item x="942"/>
+        <item x="943"/>
+        <item x="968"/>
+        <item x="969"/>
+        <item x="970"/>
+        <item x="971"/>
+        <item x="972"/>
+        <item x="973"/>
+        <item x="974"/>
+        <item x="975"/>
+        <item x="976"/>
+        <item x="960"/>
+        <item x="977"/>
+        <item x="978"/>
+        <item x="979"/>
+        <item x="980"/>
+        <item x="981"/>
+        <item x="982"/>
+        <item x="961"/>
+        <item x="962"/>
+        <item x="963"/>
+        <item x="964"/>
+        <item x="965"/>
+        <item x="966"/>
+        <item x="967"/>
+        <item x="991"/>
+        <item x="992"/>
+        <item x="993"/>
+        <item x="994"/>
+        <item x="995"/>
+        <item x="996"/>
+        <item x="997"/>
+        <item x="998"/>
+        <item x="999"/>
+        <item x="1000"/>
+        <item x="983"/>
+        <item x="1001"/>
+        <item x="1002"/>
+        <item x="1003"/>
+        <item x="1004"/>
+        <item x="1005"/>
+        <item x="1006"/>
+        <item x="984"/>
+        <item x="985"/>
+        <item x="986"/>
+        <item x="987"/>
+        <item x="988"/>
+        <item x="989"/>
+        <item x="990"/>
+        <item x="100"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="101"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="125"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="143"/>
+        <item x="126"/>
+        <item x="144"/>
+        <item x="145"/>
+        <item x="146"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="149"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="150"/>
+        <item x="159"/>
+        <item x="160"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="163"/>
+        <item x="164"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="151"/>
+        <item x="167"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="170"/>
+        <item x="171"/>
+        <item x="172"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="154"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="173"/>
+        <item x="182"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="185"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="190"/>
+        <item x="191"/>
+        <item x="174"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="194"/>
+        <item x="195"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="177"/>
+        <item x="178"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="206"/>
+        <item x="207"/>
+        <item x="208"/>
+        <item x="209"/>
+        <item x="210"/>
+        <item x="211"/>
+        <item x="212"/>
+        <item x="213"/>
+        <item x="214"/>
+        <item x="215"/>
+        <item x="198"/>
+        <item x="216"/>
+        <item x="217"/>
+        <item x="218"/>
+        <item x="219"/>
+        <item x="220"/>
+        <item x="199"/>
+        <item x="200"/>
+        <item x="201"/>
+        <item x="202"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item x="205"/>
+        <item x="1007"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField compact="0" showAll="0"/>
     <pivotField axis="axisPage" compact="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="11">
@@ -23600,7 +24612,257 @@
     </pivotField>
     <pivotField compact="0" showAll="0"/>
     <pivotField compact="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" showAll="0">
+      <items count="247">
+        <item x="164"/>
+        <item x="198"/>
+        <item x="221"/>
+        <item x="87"/>
+        <item x="224"/>
+        <item x="79"/>
+        <item x="244"/>
+        <item x="144"/>
+        <item x="234"/>
+        <item x="197"/>
+        <item x="47"/>
+        <item x="133"/>
+        <item x="153"/>
+        <item x="126"/>
+        <item x="186"/>
+        <item x="115"/>
+        <item x="148"/>
+        <item x="190"/>
+        <item x="57"/>
+        <item x="132"/>
+        <item x="21"/>
+        <item x="206"/>
+        <item x="5"/>
+        <item x="171"/>
+        <item x="52"/>
+        <item x="210"/>
+        <item x="233"/>
+        <item x="89"/>
+        <item x="151"/>
+        <item x="80"/>
+        <item x="172"/>
+        <item x="54"/>
+        <item x="147"/>
+        <item x="175"/>
+        <item x="178"/>
+        <item x="48"/>
+        <item x="20"/>
+        <item x="163"/>
+        <item x="98"/>
+        <item x="104"/>
+        <item x="176"/>
+        <item x="127"/>
+        <item x="55"/>
+        <item x="32"/>
+        <item x="61"/>
+        <item x="211"/>
+        <item x="100"/>
+        <item x="45"/>
+        <item x="212"/>
+        <item x="136"/>
+        <item x="207"/>
+        <item x="154"/>
+        <item x="64"/>
+        <item x="6"/>
+        <item x="158"/>
+        <item x="83"/>
+        <item x="111"/>
+        <item x="122"/>
+        <item x="203"/>
+        <item x="140"/>
+        <item x="194"/>
+        <item x="142"/>
+        <item x="22"/>
+        <item x="182"/>
+        <item x="26"/>
+        <item x="193"/>
+        <item x="118"/>
+        <item x="213"/>
+        <item x="12"/>
+        <item x="66"/>
+        <item x="187"/>
+        <item x="43"/>
+        <item x="220"/>
+        <item x="130"/>
+        <item x="59"/>
+        <item x="229"/>
+        <item x="19"/>
+        <item x="93"/>
+        <item x="71"/>
+        <item x="2"/>
+        <item x="107"/>
+        <item x="191"/>
+        <item x="173"/>
+        <item x="60"/>
+        <item x="23"/>
+        <item x="237"/>
+        <item x="58"/>
+        <item x="161"/>
+        <item x="31"/>
+        <item x="119"/>
+        <item x="113"/>
+        <item x="195"/>
+        <item x="17"/>
+        <item x="75"/>
+        <item x="242"/>
+        <item x="204"/>
+        <item x="7"/>
+        <item x="101"/>
+        <item x="170"/>
+        <item x="216"/>
+        <item x="77"/>
+        <item x="185"/>
+        <item x="8"/>
+        <item x="183"/>
+        <item x="232"/>
+        <item x="223"/>
+        <item x="1"/>
+        <item x="92"/>
+        <item x="46"/>
+        <item x="192"/>
+        <item x="155"/>
+        <item x="28"/>
+        <item x="156"/>
+        <item x="157"/>
+        <item x="103"/>
+        <item x="42"/>
+        <item x="143"/>
+        <item x="138"/>
+        <item x="181"/>
+        <item x="139"/>
+        <item x="112"/>
+        <item x="72"/>
+        <item x="219"/>
+        <item x="13"/>
+        <item x="69"/>
+        <item x="208"/>
+        <item x="123"/>
+        <item x="88"/>
+        <item x="0"/>
+        <item x="217"/>
+        <item x="24"/>
+        <item x="95"/>
+        <item x="179"/>
+        <item x="15"/>
+        <item x="209"/>
+        <item x="90"/>
+        <item x="236"/>
+        <item x="62"/>
+        <item x="238"/>
+        <item x="99"/>
+        <item x="9"/>
+        <item x="63"/>
+        <item x="96"/>
+        <item x="162"/>
+        <item x="33"/>
+        <item x="53"/>
+        <item x="73"/>
+        <item x="137"/>
+        <item x="27"/>
+        <item x="49"/>
+        <item x="121"/>
+        <item x="94"/>
+        <item x="35"/>
+        <item x="228"/>
+        <item x="38"/>
+        <item x="76"/>
+        <item x="91"/>
+        <item x="84"/>
+        <item x="202"/>
+        <item x="37"/>
+        <item x="40"/>
+        <item x="44"/>
+        <item x="117"/>
+        <item x="145"/>
+        <item x="199"/>
+        <item x="141"/>
+        <item x="215"/>
+        <item x="152"/>
+        <item x="4"/>
+        <item x="108"/>
+        <item x="120"/>
+        <item x="85"/>
+        <item x="135"/>
+        <item x="166"/>
+        <item x="41"/>
+        <item x="34"/>
+        <item x="65"/>
+        <item x="159"/>
+        <item x="125"/>
+        <item x="97"/>
+        <item x="124"/>
+        <item x="114"/>
+        <item x="16"/>
+        <item x="50"/>
+        <item x="235"/>
+        <item x="86"/>
+        <item x="70"/>
+        <item x="149"/>
+        <item x="78"/>
+        <item x="169"/>
+        <item x="109"/>
+        <item x="56"/>
+        <item x="227"/>
+        <item x="131"/>
+        <item x="134"/>
+        <item x="129"/>
+        <item x="150"/>
+        <item x="67"/>
+        <item x="110"/>
+        <item x="218"/>
+        <item x="230"/>
+        <item x="222"/>
+        <item x="74"/>
+        <item x="241"/>
+        <item x="68"/>
+        <item x="214"/>
+        <item x="82"/>
+        <item x="116"/>
+        <item x="14"/>
+        <item x="168"/>
+        <item x="196"/>
+        <item x="201"/>
+        <item x="226"/>
+        <item x="10"/>
+        <item x="18"/>
+        <item x="39"/>
+        <item x="102"/>
+        <item x="167"/>
+        <item x="11"/>
+        <item x="81"/>
+        <item x="189"/>
+        <item x="36"/>
+        <item x="146"/>
+        <item x="29"/>
+        <item x="174"/>
+        <item x="25"/>
+        <item x="240"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="30"/>
+        <item x="51"/>
+        <item x="184"/>
+        <item x="188"/>
+        <item x="160"/>
+        <item x="165"/>
+        <item x="180"/>
+        <item x="3"/>
+        <item x="128"/>
+        <item x="239"/>
+        <item x="200"/>
+        <item x="177"/>
+        <item x="225"/>
+        <item x="205"/>
+        <item x="243"/>
+        <item x="231"/>
+        <item x="245"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisPage" compact="0" showAll="0">
       <items count="3">
         <item x="0"/>
@@ -24152,7 +25414,7 @@
   <dimension ref="A1:AH10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -24465,7 +25727,7 @@
   <dimension ref="A1:L1008"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B$1:J$1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14"/>

</xml_diff>